<commit_message>
Rectifying a value in org dataset and Adding utility for handling different types of evaluations
</commit_message>
<xml_diff>
--- a/DATASET/DATASET.xlsx
+++ b/DATASET/DATASET.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainashastri/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainashastri/Desktop/239/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Org" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
   <si>
     <t>USERS</t>
   </si>
@@ -153,6 +153,12 @@
   <si>
     <t>Focus</t>
   </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -213,16 +219,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM44"/>
+  <dimension ref="A1:AN44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AL44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,7 +532,7 @@
     <col min="37" max="37" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,8 +650,9 @@
       <c r="AM1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AN1" s="1"/>
     </row>
-    <row r="2" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>792</v>
       </c>
@@ -734,7 +754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>474</v>
       </c>
@@ -838,7 +858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>831</v>
       </c>
@@ -951,8 +971,9 @@
       <c r="AL4" s="1">
         <v>4</v>
       </c>
+      <c r="AN4" s="6"/>
     </row>
-    <row r="5" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>204</v>
       </c>
@@ -1058,7 +1079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>62</v>
       </c>
@@ -1128,7 +1149,7 @@
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
     </row>
-    <row r="7" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>479</v>
       </c>
@@ -1206,7 +1227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>224</v>
       </c>
@@ -1286,7 +1307,7 @@
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
     </row>
-    <row r="9" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>75</v>
       </c>
@@ -1362,7 +1383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>686</v>
       </c>
@@ -1426,7 +1447,7 @@
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
     </row>
-    <row r="11" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>519</v>
       </c>
@@ -1492,7 +1513,7 @@
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
     </row>
-    <row r="12" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>253</v>
       </c>
@@ -1588,7 +1609,7 @@
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
     </row>
-    <row r="13" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>263</v>
       </c>
@@ -1674,7 +1695,7 @@
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
     </row>
-    <row r="14" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>616</v>
       </c>
@@ -1742,7 +1763,7 @@
       </c>
       <c r="AL14" s="2"/>
     </row>
-    <row r="15" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>331</v>
       </c>
@@ -1806,7 +1827,7 @@
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
     </row>
-    <row r="16" spans="1:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>355</v>
       </c>
@@ -3529,9 +3550,7 @@
       <c r="AD40" s="1">
         <v>4</v>
       </c>
-      <c r="AE40" s="1">
-        <v>0</v>
-      </c>
+      <c r="AE40" s="1"/>
       <c r="AF40" s="1">
         <v>4</v>
       </c>
@@ -3848,8 +3867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView topLeftCell="W20" workbookViewId="0">
+      <selection activeCell="AM40" sqref="AM40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7182,9 +7201,7 @@
       <c r="AD40" s="1">
         <v>4</v>
       </c>
-      <c r="AE40" s="1">
-        <v>0</v>
-      </c>
+      <c r="AE40" s="1"/>
       <c r="AF40" s="1">
         <v>4</v>
       </c>
@@ -7541,10 +7558,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL44"/>
+  <dimension ref="A1:AO44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7556,7 +7573,7 @@
     <col min="37" max="37" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7671,8 +7688,14 @@
       <c r="AL1" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="AM1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>792</v>
       </c>
@@ -7824,8 +7847,15 @@
         <f>IF(Average!AL2&gt;0,SUM(Average!AL2,Average!$AN$2),"")</f>
         <v>-1.1333333333333337</v>
       </c>
+      <c r="AN2">
+        <f>COUNTIF(B2:AL2,"&gt;0")+COUNTIF(B2:AL2,"&lt;0")+COUNTIF(B2:AL2,"=0")</f>
+        <v>30</v>
+      </c>
+      <c r="AO2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>474</v>
       </c>
@@ -7977,8 +8007,15 @@
         <f>IF(Average!AL3&gt;0,SUM(Average!AL3,Average!$AN$3),"")</f>
         <v>-9.6774193548387011E-2</v>
       </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN44" si="0">COUNTIF(B3:AL3,"&gt;0")+COUNTIF(B3:AL3,"&lt;0")+COUNTIF(B3:AL3,"=0")</f>
+        <v>31</v>
+      </c>
+      <c r="AO3">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>831</v>
       </c>
@@ -8130,314 +8167,335 @@
         <f>IF(Average!AL4&gt;0,SUM(Average!AL4,Average!$AN$4),"")</f>
         <v>0</v>
       </c>
+      <c r="AN4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AO4">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>204</v>
       </c>
       <c r="B5" s="1">
-        <f>IF(Average!B5&gt;0,SUM(Average!B5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!B5&gt;0,SUM(Average!B5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="C5" s="1">
-        <f>IF(Average!C5&gt;0,SUM(Average!C5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!C5&gt;0,SUM(Average!C5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="D5" s="1">
-        <f>IF(Average!D5&gt;0,SUM(Average!D5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!D5&gt;0,SUM(Average!D5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="E5" s="1">
-        <f>IF(Average!E5&gt;0,SUM(Average!E5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!E5&gt;0,SUM(Average!E5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="F5" s="1">
-        <f>IF(Average!F5&gt;0,SUM(Average!F5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!F5&gt;0,SUM(Average!F5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="G5" s="1">
-        <f>IF(Average!G5&gt;0,SUM(Average!G5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!G5&gt;0,SUM(Average!G5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="H5" s="1">
-        <f>IF(Average!H5&gt;0,SUM(Average!H5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!H5&gt;0,SUM(Average!H5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="I5" s="1">
-        <f>IF(Average!I5&gt;0,SUM(Average!I5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!I5&gt;0,SUM(Average!I5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="J5" s="1">
-        <f>IF(Average!J5&gt;0,SUM(Average!J5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!J5&gt;0,SUM(Average!J5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="K5" s="1">
-        <f>IF(Average!K5&gt;0,SUM(Average!K5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!K5&gt;0,SUM(Average!K5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="L5" s="1">
-        <f>IF(Average!L5&gt;0,SUM(Average!L5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!L5&gt;0,SUM(Average!L5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="M5" s="1">
-        <f>IF(Average!M5&gt;0,SUM(Average!M5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!M5&gt;0,SUM(Average!M5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="N5" s="1">
-        <f>IF(Average!N5&gt;0,SUM(Average!N5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!N5&gt;0,SUM(Average!N5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="O5" s="1">
-        <f>IF(Average!O5&gt;0,SUM(Average!O5,Average!$AN$4),"")</f>
-        <v>-2</v>
+        <f>IF(Average!O5&gt;0,SUM(Average!O5,Average!$AN$5),"")</f>
+        <v>-1.59375</v>
       </c>
       <c r="P5" s="1">
-        <f>IF(Average!P5&gt;0,SUM(Average!P5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!P5&gt;0,SUM(Average!P5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="Q5" s="1">
-        <f>IF(Average!Q5&gt;0,SUM(Average!Q5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!Q5&gt;0,SUM(Average!Q5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="R5" s="1">
-        <f>IF(Average!R5&gt;0,SUM(Average!R5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!R5&gt;0,SUM(Average!R5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="S5" s="1" t="str">
-        <f>IF(Average!S5&gt;0,SUM(Average!S5,Average!$AN$4),"")</f>
+        <f>IF(Average!S5&gt;0,SUM(Average!S5,Average!$AN$5),"")</f>
         <v/>
       </c>
       <c r="T5" s="1" t="str">
-        <f>IF(Average!T5&gt;0,SUM(Average!T5,Average!$AN$4),"")</f>
+        <f>IF(Average!T5&gt;0,SUM(Average!T5,Average!$AN$5),"")</f>
         <v/>
       </c>
       <c r="U5" s="1">
-        <f>IF(Average!U5&gt;0,SUM(Average!U5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!U5&gt;0,SUM(Average!U5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="V5" s="1" t="str">
-        <f>IF(Average!V5&gt;0,SUM(Average!V5,Average!$AN$4),"")</f>
+        <f>IF(Average!V5&gt;0,SUM(Average!V5,Average!$AN$5),"")</f>
         <v/>
       </c>
       <c r="W5" s="1">
-        <f>IF(Average!W5&gt;0,SUM(Average!W5,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!W5&gt;0,SUM(Average!W5,Average!$AN$5),"")</f>
+        <v>1.40625</v>
       </c>
       <c r="X5" s="1">
-        <f>IF(Average!X5&gt;0,SUM(Average!X5,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!X5&gt;0,SUM(Average!X5,Average!$AN$5),"")</f>
+        <v>1.40625</v>
       </c>
       <c r="Y5" s="1">
-        <f>IF(Average!Y5&gt;0,SUM(Average!Y5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!Y5&gt;0,SUM(Average!Y5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="Z5" s="1">
-        <f>IF(Average!Z5&gt;0,SUM(Average!Z5,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!Z5&gt;0,SUM(Average!Z5,Average!$AN$5),"")</f>
+        <v>1.40625</v>
       </c>
       <c r="AA5" s="1">
-        <f>IF(Average!AA5&gt;0,SUM(Average!AA5,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!AA5&gt;0,SUM(Average!AA5,Average!$AN$5),"")</f>
+        <v>1.40625</v>
       </c>
       <c r="AB5" s="1">
-        <f>IF(Average!AB5&gt;0,SUM(Average!AB5,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!AB5&gt;0,SUM(Average!AB5,Average!$AN$5),"")</f>
+        <v>1.40625</v>
       </c>
       <c r="AC5" s="1" t="str">
-        <f>IF(Average!AC5&gt;0,SUM(Average!AC5,Average!$AN$4),"")</f>
+        <f>IF(Average!AC5&gt;0,SUM(Average!AC5,Average!$AN$5),"")</f>
         <v/>
       </c>
       <c r="AD5" s="1" t="str">
-        <f>IF(Average!AD5&gt;0,SUM(Average!AD5,Average!$AN$4),"")</f>
+        <f>IF(Average!AD5&gt;0,SUM(Average!AD5,Average!$AN$5),"")</f>
         <v/>
       </c>
       <c r="AE5" s="1">
-        <f>IF(Average!AE5&gt;0,SUM(Average!AE5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!AE5&gt;0,SUM(Average!AE5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
       </c>
       <c r="AF5" s="1">
-        <f>IF(Average!AF5&gt;0,SUM(Average!AF5,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!AF5&gt;0,SUM(Average!AF5,Average!$AN$5),"")</f>
+        <v>0.40625</v>
       </c>
       <c r="AG5" s="1">
-        <f>IF(Average!AG5&gt;0,SUM(Average!AG5,Average!$AN$4),"")</f>
-        <v>-2</v>
+        <f>IF(Average!AG5&gt;0,SUM(Average!AG5,Average!$AN$5),"")</f>
+        <v>-1.59375</v>
       </c>
       <c r="AH5" s="1">
-        <f>IF(Average!AH5&gt;0,SUM(Average!AH5,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!AH5&gt;0,SUM(Average!AH5,Average!$AN$5),"")</f>
+        <v>1.40625</v>
       </c>
       <c r="AI5" s="1">
-        <f>IF(Average!AI5&gt;0,SUM(Average!AI5,Average!$AN$4),"")</f>
-        <v>-3</v>
+        <f>IF(Average!AI5&gt;0,SUM(Average!AI5,Average!$AN$5),"")</f>
+        <v>-2.59375</v>
       </c>
       <c r="AJ5" s="1">
-        <f>IF(Average!AJ5&gt;0,SUM(Average!AJ5,Average!$AN$4),"")</f>
-        <v>-2</v>
+        <f>IF(Average!AJ5&gt;0,SUM(Average!AJ5,Average!$AN$5),"")</f>
+        <v>-1.59375</v>
       </c>
       <c r="AK5" s="1">
-        <f>IF(Average!AK5&gt;0,SUM(Average!AK5,Average!$AN$4),"")</f>
-        <v>-2</v>
+        <f>IF(Average!AK5&gt;0,SUM(Average!AK5,Average!$AN$5),"")</f>
+        <v>-1.59375</v>
       </c>
       <c r="AL5" s="1">
-        <f>IF(Average!AL5&gt;0,SUM(Average!AL5,Average!$AN$4),"")</f>
-        <v>-1</v>
+        <f>IF(Average!AL5&gt;0,SUM(Average!AL5,Average!$AN$5),"")</f>
+        <v>-0.59375</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AO5">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>62</v>
       </c>
       <c r="B6" s="1">
-        <f>IF(Average!B6&gt;0,SUM(Average!B6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!B6&gt;0,SUM(Average!B6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>IF(Average!C6&gt;0,SUM(Average!C6,Average!$AN$4),"")</f>
+        <f>IF(Average!C6&gt;0,SUM(Average!C6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="D6" s="1">
-        <f>IF(Average!D6&gt;0,SUM(Average!D6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!D6&gt;0,SUM(Average!D6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="E6" s="1">
-        <f>IF(Average!E6&gt;0,SUM(Average!E6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!E6&gt;0,SUM(Average!E6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="F6" s="1">
-        <f>IF(Average!F6&gt;0,SUM(Average!F6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!F6&gt;0,SUM(Average!F6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="G6" s="1">
-        <f>IF(Average!G6&gt;0,SUM(Average!G6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!G6&gt;0,SUM(Average!G6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF(Average!H6&gt;0,SUM(Average!H6,Average!$AN$4),"")</f>
+        <f>IF(Average!H6&gt;0,SUM(Average!H6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="I6" s="1">
-        <f>IF(Average!I6&gt;0,SUM(Average!I6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!I6&gt;0,SUM(Average!I6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="J6" s="1" t="str">
-        <f>IF(Average!J6&gt;0,SUM(Average!J6,Average!$AN$4),"")</f>
+        <f>IF(Average!J6&gt;0,SUM(Average!J6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="K6" s="1" t="str">
-        <f>IF(Average!K6&gt;0,SUM(Average!K6,Average!$AN$4),"")</f>
+        <f>IF(Average!K6&gt;0,SUM(Average!K6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="L6" s="1" t="str">
-        <f>IF(Average!L6&gt;0,SUM(Average!L6,Average!$AN$4),"")</f>
+        <f>IF(Average!L6&gt;0,SUM(Average!L6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="M6" s="1">
-        <f>IF(Average!M6&gt;0,SUM(Average!M6,Average!$AN$4),"")</f>
-        <v>0</v>
+        <f>IF(Average!M6&gt;0,SUM(Average!M6,Average!$AN$6),"")</f>
+        <v>-0.64285714285714324</v>
       </c>
       <c r="N6" s="1">
-        <f>IF(Average!N6&gt;0,SUM(Average!N6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!N6&gt;0,SUM(Average!N6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="O6" s="1">
-        <f>IF(Average!O6&gt;0,SUM(Average!O6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!O6&gt;0,SUM(Average!O6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="P6" s="1" t="str">
-        <f>IF(Average!P6&gt;0,SUM(Average!P6,Average!$AN$4),"")</f>
+        <f>IF(Average!P6&gt;0,SUM(Average!P6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="Q6" s="1" t="str">
-        <f>IF(Average!Q6&gt;0,SUM(Average!Q6,Average!$AN$4),"")</f>
+        <f>IF(Average!Q6&gt;0,SUM(Average!Q6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="R6" s="1" t="str">
-        <f>IF(Average!R6&gt;0,SUM(Average!R6,Average!$AN$4),"")</f>
+        <f>IF(Average!R6&gt;0,SUM(Average!R6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="S6" s="1" t="str">
-        <f>IF(Average!S6&gt;0,SUM(Average!S6,Average!$AN$4),"")</f>
+        <f>IF(Average!S6&gt;0,SUM(Average!S6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="T6" s="1">
-        <f>IF(Average!T6&gt;0,SUM(Average!T6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!T6&gt;0,SUM(Average!T6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="U6" s="1">
-        <f>IF(Average!U6&gt;0,SUM(Average!U6,Average!$AN$4),"")</f>
-        <v>-3</v>
+        <f>IF(Average!U6&gt;0,SUM(Average!U6,Average!$AN$6),"")</f>
+        <v>-3.6428571428571432</v>
       </c>
       <c r="V6" s="1" t="str">
-        <f>IF(Average!V6&gt;0,SUM(Average!V6,Average!$AN$4),"")</f>
+        <f>IF(Average!V6&gt;0,SUM(Average!V6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="W6" s="1">
-        <f>IF(Average!W6&gt;0,SUM(Average!W6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!W6&gt;0,SUM(Average!W6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="X6" s="1">
-        <f>IF(Average!X6&gt;0,SUM(Average!X6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!X6&gt;0,SUM(Average!X6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="Y6" s="1" t="str">
-        <f>IF(Average!Y6&gt;0,SUM(Average!Y6,Average!$AN$4),"")</f>
+        <f>IF(Average!Y6&gt;0,SUM(Average!Y6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="Z6" s="1" t="str">
-        <f>IF(Average!Z6&gt;0,SUM(Average!Z6,Average!$AN$4),"")</f>
+        <f>IF(Average!Z6&gt;0,SUM(Average!Z6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AA6" s="1">
-        <f>IF(Average!AA6&gt;0,SUM(Average!AA6,Average!$AN$4),"")</f>
-        <v>1</v>
+        <f>IF(Average!AA6&gt;0,SUM(Average!AA6,Average!$AN$6),"")</f>
+        <v>0.35714285714285676</v>
       </c>
       <c r="AB6" s="1" t="str">
-        <f>IF(Average!AB6&gt;0,SUM(Average!AB6,Average!$AN$4),"")</f>
+        <f>IF(Average!AB6&gt;0,SUM(Average!AB6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AC6" s="1" t="str">
-        <f>IF(Average!AC6&gt;0,SUM(Average!AC6,Average!$AN$4),"")</f>
+        <f>IF(Average!AC6&gt;0,SUM(Average!AC6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AD6" s="1" t="str">
-        <f>IF(Average!AD6&gt;0,SUM(Average!AD6,Average!$AN$4),"")</f>
+        <f>IF(Average!AD6&gt;0,SUM(Average!AD6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AE6" s="1" t="str">
-        <f>IF(Average!AE6&gt;0,SUM(Average!AE6,Average!$AN$4),"")</f>
+        <f>IF(Average!AE6&gt;0,SUM(Average!AE6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AF6" s="1" t="str">
-        <f>IF(Average!AF6&gt;0,SUM(Average!AF6,Average!$AN$4),"")</f>
+        <f>IF(Average!AF6&gt;0,SUM(Average!AF6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AG6" s="1" t="str">
-        <f>IF(Average!AG6&gt;0,SUM(Average!AG6,Average!$AN$4),"")</f>
+        <f>IF(Average!AG6&gt;0,SUM(Average!AG6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AH6" s="1" t="str">
-        <f>IF(Average!AH6&gt;0,SUM(Average!AH6,Average!$AN$4),"")</f>
+        <f>IF(Average!AH6&gt;0,SUM(Average!AH6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AI6" s="1" t="str">
-        <f>IF(Average!AI6&gt;0,SUM(Average!AI6,Average!$AN$4),"")</f>
+        <f>IF(Average!AI6&gt;0,SUM(Average!AI6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f>IF(Average!AJ6&gt;0,SUM(Average!AJ6,Average!$AN$4),"")</f>
+        <f>IF(Average!AJ6&gt;0,SUM(Average!AJ6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AK6" s="1" t="str">
-        <f>IF(Average!AK6&gt;0,SUM(Average!AK6,Average!$AN$4),"")</f>
+        <f>IF(Average!AK6&gt;0,SUM(Average!AK6,Average!$AN$6),"")</f>
         <v/>
       </c>
       <c r="AL6" s="1" t="str">
-        <f>IF(Average!AL6&gt;0,SUM(Average!AL6,Average!$AN$4),"")</f>
-        <v/>
+        <f>IF(Average!AL6&gt;0,SUM(Average!AL6,Average!$AN$6),"")</f>
+        <v/>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AO6">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>479</v>
       </c>
@@ -8589,8 +8647,15 @@
         <f>IF(Average!AL7&gt;0,SUM(Average!AL7,Average!$AN$7),"")</f>
         <v>0.77777777777777768</v>
       </c>
+      <c r="AN7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AO7">
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>224</v>
       </c>
@@ -8742,8 +8807,15 @@
         <f>IF(Average!AL8&gt;0,SUM(Average!AL8,Average!$AN$8),"")</f>
         <v/>
       </c>
+      <c r="AN8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AO8">
+        <v>19</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>75</v>
       </c>
@@ -8895,8 +8967,15 @@
         <f>IF(Average!AL9&gt;0,SUM(Average!AL9,Average!$AN$9),"")</f>
         <v>0.52941176470588225</v>
       </c>
+      <c r="AN9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AO9">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>686</v>
       </c>
@@ -9048,8 +9127,15 @@
         <f>IF(Average!AL10&gt;0,SUM(Average!AL10,Average!$AN$10),"")</f>
         <v/>
       </c>
+      <c r="AN10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AO10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="11" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>519</v>
       </c>
@@ -9201,8 +9287,15 @@
         <f>IF(Average!AL11&gt;0,SUM(Average!AL11,Average!$AN$11),"")</f>
         <v/>
       </c>
+      <c r="AN11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AO11">
+        <v>12</v>
+      </c>
     </row>
-    <row r="12" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>253</v>
       </c>
@@ -9354,161 +9447,175 @@
         <f>IF(Average!AL12&gt;0,SUM(Average!AL12,Average!$AN$12),"")</f>
         <v/>
       </c>
+      <c r="AN12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AO12">
+        <v>27</v>
+      </c>
     </row>
-    <row r="13" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>263</v>
       </c>
       <c r="B13" s="1">
-        <f>IF(Average!B13&gt;0,SUM(Average!B13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!B13&gt;0,SUM(Average!B13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="C13" s="1">
-        <f>IF(Average!C13&gt;0,SUM(Average!C13,Average!$AN$3),"")</f>
-        <v>-9.6774193548387011E-2</v>
+        <f>IF(Average!C13&gt;0,SUM(Average!C13,Average!$AN$13),"")</f>
+        <v>0.13636363636363624</v>
       </c>
       <c r="D13" s="1">
-        <f>IF(Average!D13&gt;0,SUM(Average!D13,Average!$AN$3),"")</f>
-        <v>-9.6774193548387011E-2</v>
+        <f>IF(Average!D13&gt;0,SUM(Average!D13,Average!$AN$13),"")</f>
+        <v>0.13636363636363624</v>
       </c>
       <c r="E13" s="1">
-        <f>IF(Average!E13&gt;0,SUM(Average!E13,Average!$AN$3),"")</f>
-        <v>-1.096774193548387</v>
+        <f>IF(Average!E13&gt;0,SUM(Average!E13,Average!$AN$13),"")</f>
+        <v>-0.86363636363636376</v>
       </c>
       <c r="F13" s="1">
-        <f>IF(Average!F13&gt;0,SUM(Average!F13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!F13&gt;0,SUM(Average!F13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="G13" s="1">
-        <f>IF(Average!G13&gt;0,SUM(Average!G13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!G13&gt;0,SUM(Average!G13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="H13" s="1">
-        <f>IF(Average!H13&gt;0,SUM(Average!H13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!H13&gt;0,SUM(Average!H13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="I13" s="1">
-        <f>IF(Average!I13&gt;0,SUM(Average!I13,Average!$AN$3),"")</f>
-        <v>-9.6774193548387011E-2</v>
+        <f>IF(Average!I13&gt;0,SUM(Average!I13,Average!$AN$13),"")</f>
+        <v>0.13636363636363624</v>
       </c>
       <c r="J13" s="1">
-        <f>IF(Average!J13&gt;0,SUM(Average!J13,Average!$AN$3),"")</f>
-        <v>-1.096774193548387</v>
+        <f>IF(Average!J13&gt;0,SUM(Average!J13,Average!$AN$13),"")</f>
+        <v>-0.86363636363636376</v>
       </c>
       <c r="K13" s="1">
-        <f>IF(Average!K13&gt;0,SUM(Average!K13,Average!$AN$3),"")</f>
-        <v>-2.096774193548387</v>
+        <f>IF(Average!K13&gt;0,SUM(Average!K13,Average!$AN$13),"")</f>
+        <v>-1.8636363636363638</v>
       </c>
       <c r="L13" s="1">
-        <f>IF(Average!L13&gt;0,SUM(Average!L13,Average!$AN$3),"")</f>
-        <v>-2.096774193548387</v>
+        <f>IF(Average!L13&gt;0,SUM(Average!L13,Average!$AN$13),"")</f>
+        <v>-1.8636363636363638</v>
       </c>
       <c r="M13" s="1">
-        <f>IF(Average!M13&gt;0,SUM(Average!M13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!M13&gt;0,SUM(Average!M13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="N13" s="1">
-        <f>IF(Average!N13&gt;0,SUM(Average!N13,Average!$AN$3),"")</f>
-        <v>-1.096774193548387</v>
+        <f>IF(Average!N13&gt;0,SUM(Average!N13,Average!$AN$13),"")</f>
+        <v>-0.86363636363636376</v>
       </c>
       <c r="O13" s="1">
-        <f>IF(Average!O13&gt;0,SUM(Average!O13,Average!$AN$3),"")</f>
-        <v>-2.096774193548387</v>
+        <f>IF(Average!O13&gt;0,SUM(Average!O13,Average!$AN$13),"")</f>
+        <v>-1.8636363636363638</v>
       </c>
       <c r="P13" s="1">
-        <f>IF(Average!P13&gt;0,SUM(Average!P13,Average!$AN$3),"")</f>
-        <v>-2.096774193548387</v>
+        <f>IF(Average!P13&gt;0,SUM(Average!P13,Average!$AN$13),"")</f>
+        <v>-1.8636363636363638</v>
       </c>
       <c r="Q13" s="1">
-        <f>IF(Average!Q13&gt;0,SUM(Average!Q13,Average!$AN$3),"")</f>
-        <v>-2.096774193548387</v>
+        <f>IF(Average!Q13&gt;0,SUM(Average!Q13,Average!$AN$13),"")</f>
+        <v>-1.8636363636363638</v>
       </c>
       <c r="R13" s="1">
-        <f>IF(Average!R13&gt;0,SUM(Average!R13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!R13&gt;0,SUM(Average!R13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="S13" s="1" t="str">
-        <f>IF(Average!S13&gt;0,SUM(Average!S13,Average!$AN$3),"")</f>
+        <f>IF(Average!S13&gt;0,SUM(Average!S13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="T13" s="1" t="str">
-        <f>IF(Average!T13&gt;0,SUM(Average!T13,Average!$AN$3),"")</f>
+        <f>IF(Average!T13&gt;0,SUM(Average!T13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="U13" s="1">
-        <f>IF(Average!U13&gt;0,SUM(Average!U13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!U13&gt;0,SUM(Average!U13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="V13" s="1" t="str">
-        <f>IF(Average!V13&gt;0,SUM(Average!V13,Average!$AN$3),"")</f>
+        <f>IF(Average!V13&gt;0,SUM(Average!V13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="W13" s="1" t="str">
-        <f>IF(Average!W13&gt;0,SUM(Average!W13,Average!$AN$3),"")</f>
+        <f>IF(Average!W13&gt;0,SUM(Average!W13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="X13" s="1">
-        <f>IF(Average!X13&gt;0,SUM(Average!X13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!X13&gt;0,SUM(Average!X13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="Y13" s="1">
-        <f>IF(Average!Y13&gt;0,SUM(Average!Y13,Average!$AN$3),"")</f>
-        <v>-9.6774193548387011E-2</v>
+        <f>IF(Average!Y13&gt;0,SUM(Average!Y13,Average!$AN$13),"")</f>
+        <v>0.13636363636363624</v>
       </c>
       <c r="Z13" s="1" t="str">
-        <f>IF(Average!Z13&gt;0,SUM(Average!Z13,Average!$AN$3),"")</f>
+        <f>IF(Average!Z13&gt;0,SUM(Average!Z13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AA13" s="1">
-        <f>IF(Average!AA13&gt;0,SUM(Average!AA13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!AA13&gt;0,SUM(Average!AA13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="AB13" s="1">
-        <f>IF(Average!AB13&gt;0,SUM(Average!AB13,Average!$AN$3),"")</f>
-        <v>0.90322580645161299</v>
+        <f>IF(Average!AB13&gt;0,SUM(Average!AB13,Average!$AN$13),"")</f>
+        <v>1.1363636363636362</v>
       </c>
       <c r="AC13" s="1" t="str">
-        <f>IF(Average!AC13&gt;0,SUM(Average!AC13,Average!$AN$3),"")</f>
+        <f>IF(Average!AC13&gt;0,SUM(Average!AC13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AD13" s="1" t="str">
-        <f>IF(Average!AD13&gt;0,SUM(Average!AD13,Average!$AN$3),"")</f>
+        <f>IF(Average!AD13&gt;0,SUM(Average!AD13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AE13" s="1" t="str">
-        <f>IF(Average!AE13&gt;0,SUM(Average!AE13,Average!$AN$3),"")</f>
+        <f>IF(Average!AE13&gt;0,SUM(Average!AE13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AF13" s="1" t="str">
-        <f>IF(Average!AF13&gt;0,SUM(Average!AF13,Average!$AN$3),"")</f>
+        <f>IF(Average!AF13&gt;0,SUM(Average!AF13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AG13" s="1" t="str">
-        <f>IF(Average!AG13&gt;0,SUM(Average!AG13,Average!$AN$3),"")</f>
+        <f>IF(Average!AG13&gt;0,SUM(Average!AG13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AH13" s="1" t="str">
-        <f>IF(Average!AH13&gt;0,SUM(Average!AH13,Average!$AN$3),"")</f>
+        <f>IF(Average!AH13&gt;0,SUM(Average!AH13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AI13" s="1" t="str">
-        <f>IF(Average!AI13&gt;0,SUM(Average!AI13,Average!$AN$3),"")</f>
+        <f>IF(Average!AI13&gt;0,SUM(Average!AI13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AJ13" s="1" t="str">
-        <f>IF(Average!AJ13&gt;0,SUM(Average!AJ13,Average!$AN$3),"")</f>
+        <f>IF(Average!AJ13&gt;0,SUM(Average!AJ13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AK13" s="1" t="str">
-        <f>IF(Average!AK13&gt;0,SUM(Average!AK13,Average!$AN$3),"")</f>
+        <f>IF(Average!AK13&gt;0,SUM(Average!AK13,Average!$AN$13),"")</f>
         <v/>
       </c>
       <c r="AL13" s="1" t="str">
-        <f>IF(Average!AL13&gt;0,SUM(Average!AL13,Average!$AN$3),"")</f>
-        <v/>
+        <f>IF(Average!AL13&gt;0,SUM(Average!AL13,Average!$AN$13),"")</f>
+        <v/>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AO13">
+        <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>616</v>
       </c>
@@ -9660,8 +9767,15 @@
         <f>IF(Average!AL14&gt;0,SUM(Average!AL14,Average!$AN$14),"")</f>
         <v/>
       </c>
+      <c r="AN14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AO14">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>331</v>
       </c>
@@ -9813,8 +9927,15 @@
         <f>IF(Average!AL15&gt;0,SUM(Average!AL15,Average!$AN$15),"")</f>
         <v/>
       </c>
+      <c r="AN15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AO15">
+        <v>11</v>
+      </c>
     </row>
-    <row r="16" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>355</v>
       </c>
@@ -9966,8 +10087,15 @@
         <f>IF(Average!AL16&gt;0,SUM(Average!AL16,Average!$AN$16),"")</f>
         <v/>
       </c>
+      <c r="AN16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AO16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>450</v>
       </c>
@@ -10119,8 +10247,15 @@
         <f>IF(Average!AL17&gt;0,SUM(Average!AL17,Average!$AN$17),"")</f>
         <v/>
       </c>
+      <c r="AN17">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AO17">
+        <v>17</v>
+      </c>
     </row>
-    <row r="18" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>151</v>
       </c>
@@ -10272,8 +10407,15 @@
         <f>IF(Average!AL18&gt;0,SUM(Average!AL18,Average!$AN$18),"")</f>
         <v/>
       </c>
+      <c r="AN18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AO18">
+        <v>13</v>
+      </c>
     </row>
-    <row r="19" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>52</v>
       </c>
@@ -10425,8 +10567,15 @@
         <f>IF(Average!AL19&gt;0,SUM(Average!AL19,Average!$AN$19),"")</f>
         <v/>
       </c>
+      <c r="AN19">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AO19">
+        <v>11</v>
+      </c>
     </row>
-    <row r="20" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -10578,8 +10727,15 @@
         <f>IF(Average!AL20&gt;0,SUM(Average!AL20,Average!$AN$20),"")</f>
         <v/>
       </c>
+      <c r="AN20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AO20">
+        <v>12</v>
+      </c>
     </row>
-    <row r="21" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>908</v>
       </c>
@@ -10731,8 +10887,15 @@
         <f>IF(Average!AL21&gt;0,SUM(Average!AL21,Average!$AN$21),"")</f>
         <v/>
       </c>
+      <c r="AN21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AO21">
+        <v>17</v>
+      </c>
     </row>
-    <row r="22" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>777</v>
       </c>
@@ -10884,8 +11047,15 @@
         <f>IF(Average!AL22&gt;0,SUM(Average!AL22,Average!$AN$22),"")</f>
         <v/>
       </c>
+      <c r="AN22">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AO22">
+        <v>14</v>
+      </c>
     </row>
-    <row r="23" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>292</v>
       </c>
@@ -11037,8 +11207,15 @@
         <f>IF(Average!AL23&gt;0,SUM(Average!AL23,Average!$AN$23),"")</f>
         <v/>
       </c>
+      <c r="AN23">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AO23">
+        <v>17</v>
+      </c>
     </row>
-    <row r="24" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>272</v>
       </c>
@@ -11190,8 +11367,15 @@
         <f>IF(Average!AL24&gt;0,SUM(Average!AL24,Average!$AN$24),"")</f>
         <v/>
       </c>
+      <c r="AN24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AO24">
+        <v>22</v>
+      </c>
     </row>
-    <row r="25" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>254</v>
       </c>
@@ -11343,8 +11527,15 @@
         <f>IF(Average!AL25&gt;0,SUM(Average!AL25,Average!$AN$25),"")</f>
         <v/>
       </c>
+      <c r="AN25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO25">
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>236</v>
       </c>
@@ -11496,8 +11687,15 @@
         <f>IF(Average!AL26&gt;0,SUM(Average!AL26,Average!$AN$26),"")</f>
         <v/>
       </c>
+      <c r="AN26">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AO26">
+        <v>14</v>
+      </c>
     </row>
-    <row r="27" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>445</v>
       </c>
@@ -11649,8 +11847,15 @@
         <f>IF(Average!AL27&gt;0,SUM(Average!AL27,Average!$AN$27),"")</f>
         <v>0.14705882352941169</v>
       </c>
+      <c r="AN27">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AO27">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>437</v>
       </c>
@@ -11802,8 +12007,15 @@
         <f>IF(Average!AL28&gt;0,SUM(Average!AL28,Average!$AN$28),"")</f>
         <v>-1.5625</v>
       </c>
+      <c r="AN28">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AO28">
+        <v>16</v>
+      </c>
     </row>
-    <row r="29" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>952</v>
       </c>
@@ -11955,8 +12167,15 @@
         <f>IF(Average!AL29&gt;0,SUM(Average!AL29,Average!$AN$29),"")</f>
         <v/>
       </c>
+      <c r="AN29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AO29">
+        <v>10</v>
+      </c>
     </row>
-    <row r="30" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>938</v>
       </c>
@@ -12108,8 +12327,15 @@
         <f>IF(Average!AL30&gt;0,SUM(Average!AL30,Average!$AN$30),"")</f>
         <v/>
       </c>
+      <c r="AN30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AO30">
+        <v>15</v>
+      </c>
     </row>
-    <row r="31" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>904</v>
       </c>
@@ -12261,8 +12487,15 @@
         <f>IF(Average!AL31&gt;0,SUM(Average!AL31,Average!$AN$31),"")</f>
         <v/>
       </c>
+      <c r="AN31">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AO31">
+        <v>7</v>
+      </c>
     </row>
-    <row r="32" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>953</v>
       </c>
@@ -12414,8 +12647,15 @@
         <f>IF(Average!AL32&gt;0,SUM(Average!AL32,Average!$AN$32),"")</f>
         <v/>
       </c>
+      <c r="AN32">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AO32">
+        <v>16</v>
+      </c>
     </row>
-    <row r="33" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>805</v>
       </c>
@@ -12567,8 +12807,15 @@
         <f>IF(Average!AL33&gt;0,SUM(Average!AL33,Average!$AN$33),"")</f>
         <v/>
       </c>
+      <c r="AN33">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AO33">
+        <v>22</v>
+      </c>
     </row>
-    <row r="34" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>971</v>
       </c>
@@ -12720,8 +12967,15 @@
         <f>IF(Average!AL34&gt;0,SUM(Average!AL34,Average!$AN$34),"")</f>
         <v/>
       </c>
+      <c r="AN34">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AO34">
+        <v>14</v>
+      </c>
     </row>
-    <row r="35" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>799</v>
       </c>
@@ -12873,8 +13127,15 @@
         <f>IF(Average!AL35&gt;0,SUM(Average!AL35,Average!$AN$35),"")</f>
         <v/>
       </c>
+      <c r="AN35">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AO35">
+        <v>7</v>
+      </c>
     </row>
-    <row r="36" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>697</v>
       </c>
@@ -13026,8 +13287,15 @@
         <f>IF(Average!AL36&gt;0,SUM(Average!AL36,Average!$AN$36),"")</f>
         <v/>
       </c>
+      <c r="AN36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AO36">
+        <v>9</v>
+      </c>
     </row>
-    <row r="37" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>554</v>
       </c>
@@ -13179,8 +13447,15 @@
         <f>IF(Average!AL37&gt;0,SUM(Average!AL37,Average!$AN$37),"")</f>
         <v/>
       </c>
+      <c r="AN37">
+        <f>COUNTIF(B37:AL37,"&gt;0")+COUNTIF(B37:AL37,"&lt;0")+COUNTIF(B37:AL37,"=0")</f>
+        <v>16</v>
+      </c>
+      <c r="AO37">
+        <v>16</v>
+      </c>
     </row>
-    <row r="38" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>13</v>
       </c>
@@ -13332,8 +13607,15 @@
         <f>IF(Average!AL38&gt;0,SUM(Average!AL38,Average!$AN$38),"")</f>
         <v/>
       </c>
+      <c r="AN38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AO38">
+        <v>9</v>
+      </c>
     </row>
-    <row r="39" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>339</v>
       </c>
@@ -13485,8 +13767,15 @@
         <f>IF(Average!AL39&gt;0,SUM(Average!AL39,Average!$AN$39),"")</f>
         <v/>
       </c>
+      <c r="AN39">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AO39">
+        <v>12</v>
+      </c>
     </row>
-    <row r="40" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>338</v>
       </c>
@@ -13638,8 +13927,15 @@
         <f>IF(Average!AL40&gt;0,SUM(Average!AL40,Average!$AN$40),"")</f>
         <v/>
       </c>
+      <c r="AN40">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AO40">
+        <v>13</v>
+      </c>
     </row>
-    <row r="41" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>359</v>
       </c>
@@ -13791,8 +14087,15 @@
         <f>IF(Average!AL41&gt;0,SUM(Average!AL41,Average!$AN$41),"")</f>
         <v/>
       </c>
+      <c r="AN41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AO41">
+        <v>5</v>
+      </c>
     </row>
-    <row r="42" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>179</v>
       </c>
@@ -13944,8 +14247,15 @@
         <f>IF(Average!AL42&gt;0,SUM(Average!AL42,Average!$AN$42),"")</f>
         <v/>
       </c>
+      <c r="AN42">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AO42">
+        <v>11</v>
+      </c>
     </row>
-    <row r="43" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>705</v>
       </c>
@@ -14097,8 +14407,15 @@
         <f>IF(Average!AL43&gt;0,SUM(Average!AL43,Average!$AN$43),"")</f>
         <v/>
       </c>
+      <c r="AN43">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AO43">
+        <v>27</v>
+      </c>
     </row>
-    <row r="44" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>913</v>
       </c>
@@ -14249,6 +14566,13 @@
       <c r="AL44" s="1">
         <f>IF(Average!AL44&gt;0,SUM(Average!AL44,Average!$AN$44),"")</f>
         <v>0.73684210526315752</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AO44">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 30 more users
</commit_message>
<xml_diff>
--- a/DATASET/DATASET.xlsx
+++ b/DATASET/DATASET.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainashastri/Dropbox/sts-workspace/CMPE-239/CMPE-239_RecommenderSystems/DATASET/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/balwindersingh/Downloads/CMPE-239_RecommenderSystems-master-3/DATASET/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14679,10 +14679,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN74"/>
+  <dimension ref="A1:AN104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL74" sqref="AL74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20067,6 +20067,2059 @@
         <v>4</v>
       </c>
       <c r="AK74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>3262</v>
+      </c>
+      <c r="B75" s="1">
+        <v>4</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75" s="1">
+        <v>3</v>
+      </c>
+      <c r="E75" s="1">
+        <v>5</v>
+      </c>
+      <c r="F75" s="1">
+        <v>5</v>
+      </c>
+      <c r="G75" s="1">
+        <v>4</v>
+      </c>
+      <c r="H75" s="1">
+        <v>2</v>
+      </c>
+      <c r="I75" s="1">
+        <v>2</v>
+      </c>
+      <c r="J75" s="1">
+        <v>4</v>
+      </c>
+      <c r="K75" s="1">
+        <v>5</v>
+      </c>
+      <c r="L75" s="1">
+        <v>4</v>
+      </c>
+      <c r="M75" s="1">
+        <v>4</v>
+      </c>
+      <c r="N75" s="1">
+        <v>4</v>
+      </c>
+      <c r="O75" s="1">
+        <v>5</v>
+      </c>
+      <c r="P75" s="1"/>
+      <c r="R75" s="1">
+        <v>3</v>
+      </c>
+      <c r="T75">
+        <v>3</v>
+      </c>
+      <c r="W75">
+        <v>4</v>
+      </c>
+      <c r="X75" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y75" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC75">
+        <v>5</v>
+      </c>
+      <c r="AD75">
+        <v>4</v>
+      </c>
+      <c r="AE75">
+        <v>5</v>
+      </c>
+      <c r="AF75">
+        <v>2</v>
+      </c>
+      <c r="AH75">
+        <v>4</v>
+      </c>
+      <c r="AJ75">
+        <v>1</v>
+      </c>
+      <c r="AL75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>2254</v>
+      </c>
+      <c r="B76" s="1">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2</v>
+      </c>
+      <c r="G76" s="1">
+        <v>2</v>
+      </c>
+      <c r="I76" s="1">
+        <v>5</v>
+      </c>
+      <c r="K76">
+        <v>5</v>
+      </c>
+      <c r="L76">
+        <v>4</v>
+      </c>
+      <c r="M76" s="1">
+        <v>4</v>
+      </c>
+      <c r="O76" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>3</v>
+      </c>
+      <c r="S76">
+        <v>1</v>
+      </c>
+      <c r="T76">
+        <v>4</v>
+      </c>
+      <c r="U76" s="1">
+        <v>4</v>
+      </c>
+      <c r="V76">
+        <v>3</v>
+      </c>
+      <c r="W76">
+        <v>4</v>
+      </c>
+      <c r="AA76">
+        <v>3</v>
+      </c>
+      <c r="AC76">
+        <v>5</v>
+      </c>
+      <c r="AF76">
+        <v>3</v>
+      </c>
+      <c r="AJ76">
+        <v>4</v>
+      </c>
+      <c r="AL76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>4363</v>
+      </c>
+      <c r="B77" s="1">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>4</v>
+      </c>
+      <c r="D77" s="1">
+        <v>5</v>
+      </c>
+      <c r="E77" s="1">
+        <v>5</v>
+      </c>
+      <c r="F77" s="1">
+        <v>3</v>
+      </c>
+      <c r="G77" s="1">
+        <v>4</v>
+      </c>
+      <c r="H77">
+        <v>3</v>
+      </c>
+      <c r="I77" s="1">
+        <v>5</v>
+      </c>
+      <c r="J77" s="1">
+        <v>4</v>
+      </c>
+      <c r="K77">
+        <v>4</v>
+      </c>
+      <c r="L77">
+        <v>3</v>
+      </c>
+      <c r="O77" s="1">
+        <v>4</v>
+      </c>
+      <c r="P77">
+        <v>4</v>
+      </c>
+      <c r="Q77">
+        <v>5</v>
+      </c>
+      <c r="R77">
+        <v>1</v>
+      </c>
+      <c r="T77">
+        <v>3</v>
+      </c>
+      <c r="V77">
+        <v>4</v>
+      </c>
+      <c r="X77" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y77" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z77">
+        <v>3</v>
+      </c>
+      <c r="AB77" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC77">
+        <v>5</v>
+      </c>
+      <c r="AE77">
+        <v>3</v>
+      </c>
+      <c r="AI77">
+        <v>3</v>
+      </c>
+      <c r="AJ77">
+        <v>4</v>
+      </c>
+      <c r="AK77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>5621</v>
+      </c>
+      <c r="B78" s="1">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>5</v>
+      </c>
+      <c r="D78" s="1">
+        <v>3</v>
+      </c>
+      <c r="G78" s="1">
+        <v>2</v>
+      </c>
+      <c r="I78" s="1">
+        <v>4</v>
+      </c>
+      <c r="K78">
+        <v>4</v>
+      </c>
+      <c r="M78" s="1">
+        <v>4</v>
+      </c>
+      <c r="N78">
+        <v>4</v>
+      </c>
+      <c r="O78" s="1">
+        <v>3</v>
+      </c>
+      <c r="P78">
+        <v>2</v>
+      </c>
+      <c r="U78" s="1">
+        <v>4</v>
+      </c>
+      <c r="W78">
+        <v>5</v>
+      </c>
+      <c r="Y78" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z78">
+        <v>2</v>
+      </c>
+      <c r="AC78">
+        <v>2</v>
+      </c>
+      <c r="AE78">
+        <v>3</v>
+      </c>
+      <c r="AH78">
+        <v>4</v>
+      </c>
+      <c r="AJ78">
+        <v>5</v>
+      </c>
+      <c r="AK78">
+        <v>1</v>
+      </c>
+      <c r="AL78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>3089</v>
+      </c>
+      <c r="B79" s="1">
+        <v>5</v>
+      </c>
+      <c r="E79" s="1">
+        <v>5</v>
+      </c>
+      <c r="F79" s="1">
+        <v>2</v>
+      </c>
+      <c r="G79" s="1">
+        <v>2</v>
+      </c>
+      <c r="H79">
+        <v>4</v>
+      </c>
+      <c r="I79" s="1">
+        <v>5</v>
+      </c>
+      <c r="J79" s="1">
+        <v>5</v>
+      </c>
+      <c r="L79">
+        <v>4</v>
+      </c>
+      <c r="N79">
+        <v>4</v>
+      </c>
+      <c r="O79" s="1">
+        <v>5</v>
+      </c>
+      <c r="P79">
+        <v>5</v>
+      </c>
+      <c r="Q79">
+        <v>4</v>
+      </c>
+      <c r="R79">
+        <v>1</v>
+      </c>
+      <c r="S79">
+        <v>4</v>
+      </c>
+      <c r="T79">
+        <v>5</v>
+      </c>
+      <c r="U79">
+        <v>5</v>
+      </c>
+      <c r="V79">
+        <v>4</v>
+      </c>
+      <c r="X79">
+        <v>4</v>
+      </c>
+      <c r="AA79">
+        <v>4</v>
+      </c>
+      <c r="AE79">
+        <v>3</v>
+      </c>
+      <c r="AF79">
+        <v>5</v>
+      </c>
+      <c r="AG79">
+        <v>4</v>
+      </c>
+      <c r="AH79">
+        <v>2</v>
+      </c>
+      <c r="AJ79">
+        <v>3</v>
+      </c>
+      <c r="AL79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>1089</v>
+      </c>
+      <c r="B80" s="1">
+        <v>3</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="1">
+        <v>5</v>
+      </c>
+      <c r="E80" s="1">
+        <v>4</v>
+      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="1">
+        <v>4</v>
+      </c>
+      <c r="H80" s="2"/>
+      <c r="I80" s="1">
+        <v>4</v>
+      </c>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q80">
+        <v>4</v>
+      </c>
+      <c r="S80">
+        <v>3</v>
+      </c>
+      <c r="T80">
+        <v>5</v>
+      </c>
+      <c r="Y80" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA80">
+        <v>3</v>
+      </c>
+      <c r="AC80">
+        <v>5</v>
+      </c>
+      <c r="AD80">
+        <v>5</v>
+      </c>
+      <c r="AE80">
+        <v>4</v>
+      </c>
+      <c r="AF80">
+        <v>5</v>
+      </c>
+      <c r="AG80">
+        <v>5</v>
+      </c>
+      <c r="AH80">
+        <v>3</v>
+      </c>
+      <c r="AI80">
+        <v>2</v>
+      </c>
+      <c r="AJ80">
+        <v>3</v>
+      </c>
+      <c r="AK80">
+        <v>1</v>
+      </c>
+      <c r="AL80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>5826</v>
+      </c>
+      <c r="B81" s="1">
+        <v>4</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="E81" s="1">
+        <v>5</v>
+      </c>
+      <c r="I81" s="1">
+        <v>4</v>
+      </c>
+      <c r="J81">
+        <v>4</v>
+      </c>
+      <c r="K81">
+        <v>4</v>
+      </c>
+      <c r="L81">
+        <v>3</v>
+      </c>
+      <c r="M81">
+        <v>3</v>
+      </c>
+      <c r="N81">
+        <v>3</v>
+      </c>
+      <c r="P81">
+        <v>4</v>
+      </c>
+      <c r="R81">
+        <v>1</v>
+      </c>
+      <c r="T81">
+        <v>3</v>
+      </c>
+      <c r="V81">
+        <v>4</v>
+      </c>
+      <c r="X81">
+        <v>3</v>
+      </c>
+      <c r="Z81">
+        <v>4</v>
+      </c>
+      <c r="AA81">
+        <v>4</v>
+      </c>
+      <c r="AB81">
+        <v>4</v>
+      </c>
+      <c r="AC81">
+        <v>5</v>
+      </c>
+      <c r="AE81">
+        <v>5</v>
+      </c>
+      <c r="AF81">
+        <v>5</v>
+      </c>
+      <c r="AI81">
+        <v>4</v>
+      </c>
+      <c r="AK81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>9912</v>
+      </c>
+      <c r="B82" s="1">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1">
+        <v>5</v>
+      </c>
+      <c r="D82" s="1">
+        <v>3</v>
+      </c>
+      <c r="E82" s="1">
+        <v>5</v>
+      </c>
+      <c r="F82" s="1">
+        <v>5</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+      <c r="I82" s="1">
+        <v>1</v>
+      </c>
+      <c r="J82" s="1">
+        <v>5</v>
+      </c>
+      <c r="K82" s="1">
+        <v>5</v>
+      </c>
+      <c r="L82" s="1">
+        <v>3</v>
+      </c>
+      <c r="M82" s="1">
+        <v>4</v>
+      </c>
+      <c r="N82" s="1">
+        <v>5</v>
+      </c>
+      <c r="O82" s="1">
+        <v>5</v>
+      </c>
+      <c r="P82" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>5</v>
+      </c>
+      <c r="R82" s="1">
+        <v>4</v>
+      </c>
+      <c r="S82" s="1">
+        <v>2</v>
+      </c>
+      <c r="T82" s="1">
+        <v>2</v>
+      </c>
+      <c r="U82" s="1">
+        <v>1</v>
+      </c>
+      <c r="V82" s="1">
+        <v>3</v>
+      </c>
+      <c r="W82" s="1">
+        <v>1</v>
+      </c>
+      <c r="X82" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z82" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA82" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB82" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC82" s="2"/>
+      <c r="AD82" s="2"/>
+      <c r="AE82" s="2"/>
+      <c r="AF82" s="2"/>
+      <c r="AG82" s="2"/>
+      <c r="AH82" s="2"/>
+      <c r="AI82" s="2"/>
+      <c r="AJ82" s="2"/>
+      <c r="AK82" s="2"/>
+      <c r="AL82" s="2"/>
+    </row>
+    <row r="83" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>8552</v>
+      </c>
+      <c r="B83" s="1">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>5</v>
+      </c>
+      <c r="G83" s="1">
+        <v>5</v>
+      </c>
+      <c r="I83" s="1">
+        <v>4</v>
+      </c>
+      <c r="J83">
+        <v>4</v>
+      </c>
+      <c r="K83" s="1">
+        <v>3</v>
+      </c>
+      <c r="L83">
+        <v>2</v>
+      </c>
+      <c r="M83" s="1">
+        <v>2</v>
+      </c>
+      <c r="N83">
+        <v>4</v>
+      </c>
+      <c r="P83">
+        <v>2</v>
+      </c>
+      <c r="R83">
+        <v>4</v>
+      </c>
+      <c r="T83">
+        <v>4</v>
+      </c>
+      <c r="X83">
+        <v>4</v>
+      </c>
+      <c r="Y83">
+        <v>4</v>
+      </c>
+      <c r="Z83">
+        <v>4</v>
+      </c>
+      <c r="AB83">
+        <v>5</v>
+      </c>
+      <c r="AC83">
+        <v>5</v>
+      </c>
+      <c r="AD83">
+        <v>2</v>
+      </c>
+      <c r="AF83">
+        <v>3</v>
+      </c>
+      <c r="AG83">
+        <v>3</v>
+      </c>
+      <c r="AH83">
+        <v>4</v>
+      </c>
+      <c r="AI83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>3311</v>
+      </c>
+      <c r="B84" s="1">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+      <c r="F84">
+        <v>5</v>
+      </c>
+      <c r="H84">
+        <v>4</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>2</v>
+      </c>
+      <c r="M84">
+        <v>3</v>
+      </c>
+      <c r="N84">
+        <v>3</v>
+      </c>
+      <c r="O84" s="1">
+        <v>4</v>
+      </c>
+      <c r="P84">
+        <v>5</v>
+      </c>
+      <c r="Q84">
+        <v>5</v>
+      </c>
+      <c r="S84">
+        <v>3</v>
+      </c>
+      <c r="U84">
+        <v>4</v>
+      </c>
+      <c r="V84">
+        <v>4</v>
+      </c>
+      <c r="X84">
+        <v>4</v>
+      </c>
+      <c r="AA84">
+        <v>4</v>
+      </c>
+      <c r="AC84">
+        <v>3</v>
+      </c>
+      <c r="AE84">
+        <v>3</v>
+      </c>
+      <c r="AH84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>5234</v>
+      </c>
+      <c r="B85" s="1">
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="G85" s="1">
+        <v>3</v>
+      </c>
+      <c r="I85" s="1">
+        <v>3</v>
+      </c>
+      <c r="K85">
+        <v>5</v>
+      </c>
+      <c r="M85">
+        <v>1</v>
+      </c>
+      <c r="N85">
+        <v>2</v>
+      </c>
+      <c r="O85">
+        <v>4</v>
+      </c>
+      <c r="P85">
+        <v>3</v>
+      </c>
+      <c r="Q85">
+        <v>5</v>
+      </c>
+      <c r="T85">
+        <v>4</v>
+      </c>
+      <c r="U85">
+        <v>3</v>
+      </c>
+      <c r="V85">
+        <v>5</v>
+      </c>
+      <c r="W85">
+        <v>3</v>
+      </c>
+      <c r="X85">
+        <v>1</v>
+      </c>
+      <c r="Y85">
+        <v>2</v>
+      </c>
+      <c r="AC85">
+        <v>4</v>
+      </c>
+      <c r="AD85">
+        <v>5</v>
+      </c>
+      <c r="AE85">
+        <v>3</v>
+      </c>
+      <c r="AF85">
+        <v>5</v>
+      </c>
+      <c r="AG85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>9680</v>
+      </c>
+      <c r="B86" s="1">
+        <v>5</v>
+      </c>
+      <c r="E86">
+        <v>5</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="G86" s="1">
+        <v>3</v>
+      </c>
+      <c r="H86">
+        <v>4</v>
+      </c>
+      <c r="I86" s="1">
+        <v>4</v>
+      </c>
+      <c r="J86">
+        <v>5</v>
+      </c>
+      <c r="K86">
+        <v>4</v>
+      </c>
+      <c r="L86">
+        <v>3</v>
+      </c>
+      <c r="M86">
+        <v>3</v>
+      </c>
+      <c r="N86">
+        <v>4</v>
+      </c>
+      <c r="P86">
+        <v>2</v>
+      </c>
+      <c r="Q86">
+        <v>3</v>
+      </c>
+      <c r="R86">
+        <v>4</v>
+      </c>
+      <c r="S86">
+        <v>4</v>
+      </c>
+      <c r="W86">
+        <v>2</v>
+      </c>
+      <c r="X86">
+        <v>4</v>
+      </c>
+      <c r="Y86">
+        <v>3</v>
+      </c>
+      <c r="Z86">
+        <v>4</v>
+      </c>
+      <c r="AA86">
+        <v>4</v>
+      </c>
+      <c r="AB86">
+        <v>4</v>
+      </c>
+      <c r="AD86">
+        <v>4</v>
+      </c>
+      <c r="AE86">
+        <v>4</v>
+      </c>
+      <c r="AF86">
+        <v>3</v>
+      </c>
+      <c r="AG86">
+        <v>4</v>
+      </c>
+      <c r="AI86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>9022</v>
+      </c>
+      <c r="B87" s="1">
+        <v>3</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="H87">
+        <v>4</v>
+      </c>
+      <c r="I87" s="1">
+        <v>3</v>
+      </c>
+      <c r="J87">
+        <v>4</v>
+      </c>
+      <c r="N87">
+        <v>4</v>
+      </c>
+      <c r="P87">
+        <v>3</v>
+      </c>
+      <c r="R87">
+        <v>1</v>
+      </c>
+      <c r="S87">
+        <v>4</v>
+      </c>
+      <c r="T87">
+        <v>5</v>
+      </c>
+      <c r="U87">
+        <v>3</v>
+      </c>
+      <c r="V87">
+        <v>5</v>
+      </c>
+      <c r="W87">
+        <v>2</v>
+      </c>
+      <c r="X87">
+        <v>4</v>
+      </c>
+      <c r="AA87">
+        <v>3</v>
+      </c>
+      <c r="AC87">
+        <v>5</v>
+      </c>
+      <c r="AE87">
+        <v>5</v>
+      </c>
+      <c r="AG87">
+        <v>5</v>
+      </c>
+      <c r="AH87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>3809</v>
+      </c>
+      <c r="B88" s="1">
+        <v>5</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="G88" s="1">
+        <v>3</v>
+      </c>
+      <c r="H88">
+        <v>4</v>
+      </c>
+      <c r="I88" s="1">
+        <v>5</v>
+      </c>
+      <c r="J88">
+        <v>4</v>
+      </c>
+      <c r="K88">
+        <v>3</v>
+      </c>
+      <c r="M88">
+        <v>4</v>
+      </c>
+      <c r="N88">
+        <v>4</v>
+      </c>
+      <c r="O88">
+        <v>2</v>
+      </c>
+      <c r="R88">
+        <v>3</v>
+      </c>
+      <c r="S88">
+        <v>4</v>
+      </c>
+      <c r="T88">
+        <v>5</v>
+      </c>
+      <c r="U88">
+        <v>5</v>
+      </c>
+      <c r="V88">
+        <v>5</v>
+      </c>
+      <c r="W88">
+        <v>4</v>
+      </c>
+      <c r="Y88">
+        <v>4</v>
+      </c>
+      <c r="Z88">
+        <v>2</v>
+      </c>
+      <c r="AA88">
+        <v>3</v>
+      </c>
+      <c r="AB88">
+        <v>4</v>
+      </c>
+      <c r="AC88">
+        <v>4</v>
+      </c>
+      <c r="AF88">
+        <v>4</v>
+      </c>
+      <c r="AI88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>4544</v>
+      </c>
+      <c r="B89" s="1">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="H89">
+        <v>4</v>
+      </c>
+      <c r="J89">
+        <v>4</v>
+      </c>
+      <c r="K89">
+        <v>3</v>
+      </c>
+      <c r="L89">
+        <v>4</v>
+      </c>
+      <c r="M89">
+        <v>3</v>
+      </c>
+      <c r="N89">
+        <v>3</v>
+      </c>
+      <c r="O89">
+        <v>3</v>
+      </c>
+      <c r="P89">
+        <v>4</v>
+      </c>
+      <c r="Q89">
+        <v>4</v>
+      </c>
+      <c r="R89">
+        <v>3</v>
+      </c>
+      <c r="S89">
+        <v>2</v>
+      </c>
+      <c r="U89">
+        <v>1</v>
+      </c>
+      <c r="V89">
+        <v>5</v>
+      </c>
+      <c r="W89">
+        <v>5</v>
+      </c>
+      <c r="X89">
+        <v>4</v>
+      </c>
+      <c r="Y89">
+        <v>4</v>
+      </c>
+      <c r="Z89">
+        <v>4</v>
+      </c>
+      <c r="AA89">
+        <v>4</v>
+      </c>
+      <c r="AB89">
+        <v>2</v>
+      </c>
+      <c r="AC89">
+        <v>1</v>
+      </c>
+      <c r="AD89">
+        <v>4</v>
+      </c>
+      <c r="AE89">
+        <v>4</v>
+      </c>
+      <c r="AF89">
+        <v>5</v>
+      </c>
+      <c r="AG89">
+        <v>5</v>
+      </c>
+      <c r="AH89">
+        <v>4</v>
+      </c>
+      <c r="AI89">
+        <v>3</v>
+      </c>
+      <c r="AJ89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>7611</v>
+      </c>
+      <c r="B90" s="1">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90" s="1">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>4</v>
+      </c>
+      <c r="I90" s="1">
+        <v>4</v>
+      </c>
+      <c r="J90">
+        <v>3</v>
+      </c>
+      <c r="K90">
+        <v>4</v>
+      </c>
+      <c r="L90">
+        <v>5</v>
+      </c>
+      <c r="M90">
+        <v>3</v>
+      </c>
+      <c r="N90">
+        <v>4</v>
+      </c>
+      <c r="O90">
+        <v>3</v>
+      </c>
+      <c r="P90">
+        <v>4</v>
+      </c>
+      <c r="Q90">
+        <v>4</v>
+      </c>
+      <c r="R90">
+        <v>5</v>
+      </c>
+      <c r="S90">
+        <v>5</v>
+      </c>
+      <c r="T90">
+        <v>3</v>
+      </c>
+      <c r="V90">
+        <v>5</v>
+      </c>
+      <c r="W90">
+        <v>4</v>
+      </c>
+      <c r="X90">
+        <v>5</v>
+      </c>
+      <c r="Y90">
+        <v>4</v>
+      </c>
+      <c r="Z90">
+        <v>4</v>
+      </c>
+      <c r="AA90">
+        <v>2</v>
+      </c>
+      <c r="AB90">
+        <v>3</v>
+      </c>
+      <c r="AC90">
+        <v>5</v>
+      </c>
+      <c r="AE90">
+        <v>5</v>
+      </c>
+      <c r="AG90">
+        <v>3</v>
+      </c>
+      <c r="AI90">
+        <v>3</v>
+      </c>
+      <c r="AJ90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>1124</v>
+      </c>
+      <c r="B91" s="1">
+        <v>3</v>
+      </c>
+      <c r="E91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>5</v>
+      </c>
+      <c r="K91">
+        <v>2</v>
+      </c>
+      <c r="N91">
+        <v>3</v>
+      </c>
+      <c r="P91">
+        <v>2</v>
+      </c>
+      <c r="R91">
+        <v>4</v>
+      </c>
+      <c r="T91">
+        <v>4</v>
+      </c>
+      <c r="V91">
+        <v>4</v>
+      </c>
+      <c r="Y91">
+        <v>4</v>
+      </c>
+      <c r="Z91">
+        <v>5</v>
+      </c>
+      <c r="AB91">
+        <v>5</v>
+      </c>
+      <c r="AF91">
+        <v>5</v>
+      </c>
+      <c r="AI91">
+        <v>5</v>
+      </c>
+      <c r="AK91">
+        <v>5</v>
+      </c>
+      <c r="AL91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>2233</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <v>5</v>
+      </c>
+      <c r="G92">
+        <v>5</v>
+      </c>
+      <c r="J92">
+        <v>5</v>
+      </c>
+      <c r="L92">
+        <v>5</v>
+      </c>
+      <c r="N92">
+        <v>4</v>
+      </c>
+      <c r="P92">
+        <v>4</v>
+      </c>
+      <c r="R92">
+        <v>4</v>
+      </c>
+      <c r="T92">
+        <v>4</v>
+      </c>
+      <c r="W92">
+        <v>4</v>
+      </c>
+      <c r="Y92">
+        <v>4</v>
+      </c>
+      <c r="Z92">
+        <v>1</v>
+      </c>
+      <c r="AA92">
+        <v>3</v>
+      </c>
+      <c r="AB92">
+        <v>3</v>
+      </c>
+      <c r="AC92">
+        <v>3</v>
+      </c>
+      <c r="AE92">
+        <v>3</v>
+      </c>
+      <c r="AG92">
+        <v>3</v>
+      </c>
+      <c r="AI92">
+        <v>3</v>
+      </c>
+      <c r="AJ92">
+        <v>2</v>
+      </c>
+      <c r="AK92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>3344</v>
+      </c>
+      <c r="B93" s="1">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>4</v>
+      </c>
+      <c r="E93">
+        <v>4</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+      <c r="H93">
+        <v>5</v>
+      </c>
+      <c r="I93">
+        <v>4</v>
+      </c>
+      <c r="J93">
+        <v>4</v>
+      </c>
+      <c r="K93">
+        <v>4</v>
+      </c>
+      <c r="L93">
+        <v>4</v>
+      </c>
+      <c r="M93">
+        <v>3</v>
+      </c>
+      <c r="N93">
+        <v>4</v>
+      </c>
+      <c r="O93">
+        <v>3</v>
+      </c>
+      <c r="R93">
+        <v>5</v>
+      </c>
+      <c r="S93">
+        <v>5</v>
+      </c>
+      <c r="Z93">
+        <v>5</v>
+      </c>
+      <c r="AF93">
+        <v>5</v>
+      </c>
+      <c r="AH93">
+        <v>5</v>
+      </c>
+      <c r="AK93">
+        <v>2</v>
+      </c>
+      <c r="AL93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>4563</v>
+      </c>
+      <c r="B94" s="1">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>4</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+      <c r="H94">
+        <v>4</v>
+      </c>
+      <c r="I94">
+        <v>5</v>
+      </c>
+      <c r="J94">
+        <v>2</v>
+      </c>
+      <c r="L94">
+        <v>3</v>
+      </c>
+      <c r="Q94">
+        <v>3</v>
+      </c>
+      <c r="U94">
+        <v>4</v>
+      </c>
+      <c r="X94">
+        <v>5</v>
+      </c>
+      <c r="AA94">
+        <v>5</v>
+      </c>
+      <c r="AD94">
+        <v>2</v>
+      </c>
+      <c r="AF94">
+        <v>4</v>
+      </c>
+      <c r="AH94">
+        <v>3</v>
+      </c>
+      <c r="AJ94">
+        <v>3</v>
+      </c>
+      <c r="AL94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>5577</v>
+      </c>
+      <c r="D95">
+        <v>5</v>
+      </c>
+      <c r="I95">
+        <v>5</v>
+      </c>
+      <c r="K95">
+        <v>4</v>
+      </c>
+      <c r="M95">
+        <v>4</v>
+      </c>
+      <c r="N95">
+        <v>3</v>
+      </c>
+      <c r="O95">
+        <v>3</v>
+      </c>
+      <c r="Q95">
+        <v>3</v>
+      </c>
+      <c r="S95">
+        <v>2</v>
+      </c>
+      <c r="U95">
+        <v>4</v>
+      </c>
+      <c r="X95">
+        <v>4</v>
+      </c>
+      <c r="Z95">
+        <v>4</v>
+      </c>
+      <c r="AB95">
+        <v>4</v>
+      </c>
+      <c r="AG95">
+        <v>4</v>
+      </c>
+      <c r="AH95">
+        <v>4</v>
+      </c>
+      <c r="AI95">
+        <v>4</v>
+      </c>
+      <c r="AJ95">
+        <v>4</v>
+      </c>
+      <c r="AK95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>6633</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>4</v>
+      </c>
+      <c r="F96">
+        <v>4</v>
+      </c>
+      <c r="H96">
+        <v>4</v>
+      </c>
+      <c r="J96">
+        <v>4</v>
+      </c>
+      <c r="M96">
+        <v>4</v>
+      </c>
+      <c r="Q96">
+        <v>4</v>
+      </c>
+      <c r="U96">
+        <v>4</v>
+      </c>
+      <c r="V96">
+        <v>3</v>
+      </c>
+      <c r="Y96">
+        <v>5</v>
+      </c>
+      <c r="AA96">
+        <v>5</v>
+      </c>
+      <c r="AD96">
+        <v>5</v>
+      </c>
+      <c r="AF96">
+        <v>5</v>
+      </c>
+      <c r="AH96">
+        <v>5</v>
+      </c>
+      <c r="AJ96">
+        <v>5</v>
+      </c>
+      <c r="AL96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>7744</v>
+      </c>
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97">
+        <v>5</v>
+      </c>
+      <c r="F97">
+        <v>5</v>
+      </c>
+      <c r="G97">
+        <v>5</v>
+      </c>
+      <c r="I97">
+        <v>5</v>
+      </c>
+      <c r="K97">
+        <v>4</v>
+      </c>
+      <c r="M97">
+        <v>4</v>
+      </c>
+      <c r="O97">
+        <v>4</v>
+      </c>
+      <c r="Q97">
+        <v>4</v>
+      </c>
+      <c r="S97">
+        <v>4</v>
+      </c>
+      <c r="U97">
+        <v>2</v>
+      </c>
+      <c r="W97">
+        <v>2</v>
+      </c>
+      <c r="Y97">
+        <v>2</v>
+      </c>
+      <c r="AA97">
+        <v>3</v>
+      </c>
+      <c r="AC97">
+        <v>3</v>
+      </c>
+      <c r="AE97">
+        <v>3</v>
+      </c>
+      <c r="AG97">
+        <v>3</v>
+      </c>
+      <c r="AI97">
+        <v>3</v>
+      </c>
+      <c r="AL97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>8811</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="E98">
+        <v>5</v>
+      </c>
+      <c r="F98">
+        <v>4</v>
+      </c>
+      <c r="R98">
+        <v>5</v>
+      </c>
+      <c r="X98">
+        <v>4</v>
+      </c>
+      <c r="AB98">
+        <v>3</v>
+      </c>
+      <c r="AF98">
+        <v>3</v>
+      </c>
+      <c r="AI98">
+        <v>3</v>
+      </c>
+      <c r="AK98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>9927</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="G99">
+        <v>4</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+      <c r="I99">
+        <v>2</v>
+      </c>
+      <c r="J99">
+        <v>4</v>
+      </c>
+      <c r="K99">
+        <v>3</v>
+      </c>
+      <c r="L99">
+        <v>2</v>
+      </c>
+      <c r="M99">
+        <v>5</v>
+      </c>
+      <c r="N99">
+        <v>4</v>
+      </c>
+      <c r="O99">
+        <v>3</v>
+      </c>
+      <c r="P99">
+        <v>2</v>
+      </c>
+      <c r="Q99">
+        <v>4</v>
+      </c>
+      <c r="R99">
+        <v>3</v>
+      </c>
+      <c r="S99">
+        <v>5</v>
+      </c>
+      <c r="T99">
+        <v>5</v>
+      </c>
+      <c r="U99">
+        <v>3</v>
+      </c>
+      <c r="V99">
+        <v>4</v>
+      </c>
+      <c r="W99">
+        <v>2</v>
+      </c>
+      <c r="X99">
+        <v>4</v>
+      </c>
+      <c r="Y99">
+        <v>4</v>
+      </c>
+      <c r="AA99">
+        <v>4</v>
+      </c>
+      <c r="AC99">
+        <v>4</v>
+      </c>
+      <c r="AF99">
+        <v>4</v>
+      </c>
+      <c r="AG99">
+        <v>5</v>
+      </c>
+      <c r="AH99">
+        <v>3</v>
+      </c>
+      <c r="AJ99">
+        <v>3</v>
+      </c>
+      <c r="AL99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>7070</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <v>5</v>
+      </c>
+      <c r="D100">
+        <v>5</v>
+      </c>
+      <c r="G100">
+        <v>5</v>
+      </c>
+      <c r="H100">
+        <v>5</v>
+      </c>
+      <c r="K100">
+        <v>5</v>
+      </c>
+      <c r="M100">
+        <v>4</v>
+      </c>
+      <c r="N100">
+        <v>3</v>
+      </c>
+      <c r="O100">
+        <v>3</v>
+      </c>
+      <c r="R100">
+        <v>4</v>
+      </c>
+      <c r="T100">
+        <v>4</v>
+      </c>
+      <c r="V100">
+        <v>4</v>
+      </c>
+      <c r="X100">
+        <v>4</v>
+      </c>
+      <c r="Z100">
+        <v>4</v>
+      </c>
+      <c r="AB100">
+        <v>4</v>
+      </c>
+      <c r="AE100">
+        <v>4</v>
+      </c>
+      <c r="AH100">
+        <v>4</v>
+      </c>
+      <c r="AL100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>1010</v>
+      </c>
+      <c r="B101">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="E101">
+        <v>5</v>
+      </c>
+      <c r="G101">
+        <v>3</v>
+      </c>
+      <c r="J101">
+        <v>4</v>
+      </c>
+      <c r="K101">
+        <v>4</v>
+      </c>
+      <c r="M101">
+        <v>3</v>
+      </c>
+      <c r="N101">
+        <v>3</v>
+      </c>
+      <c r="P101">
+        <v>2</v>
+      </c>
+      <c r="Q101">
+        <v>2</v>
+      </c>
+      <c r="R101">
+        <v>4</v>
+      </c>
+      <c r="T101">
+        <v>5</v>
+      </c>
+      <c r="U101">
+        <v>5</v>
+      </c>
+      <c r="W101">
+        <v>4</v>
+      </c>
+      <c r="X101">
+        <v>3</v>
+      </c>
+      <c r="Y101">
+        <v>2</v>
+      </c>
+      <c r="Z101">
+        <v>1</v>
+      </c>
+      <c r="AA101">
+        <v>4</v>
+      </c>
+      <c r="AC101">
+        <v>4</v>
+      </c>
+      <c r="AE101">
+        <v>5</v>
+      </c>
+      <c r="AG101">
+        <v>3</v>
+      </c>
+      <c r="AH101">
+        <v>3</v>
+      </c>
+      <c r="AI101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B102">
+        <v>5</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="E102">
+        <v>4</v>
+      </c>
+      <c r="G102">
+        <v>2</v>
+      </c>
+      <c r="I102">
+        <v>4</v>
+      </c>
+      <c r="J102">
+        <v>4</v>
+      </c>
+      <c r="K102">
+        <v>3</v>
+      </c>
+      <c r="O102">
+        <v>2</v>
+      </c>
+      <c r="P102">
+        <v>4</v>
+      </c>
+      <c r="W102">
+        <v>4</v>
+      </c>
+      <c r="AD102">
+        <v>5</v>
+      </c>
+      <c r="AJ102">
+        <v>5</v>
+      </c>
+      <c r="AL102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>2121</v>
+      </c>
+      <c r="C103">
+        <v>5</v>
+      </c>
+      <c r="F103">
+        <v>4</v>
+      </c>
+      <c r="L103">
+        <v>3</v>
+      </c>
+      <c r="R103">
+        <v>4</v>
+      </c>
+      <c r="V103">
+        <v>2</v>
+      </c>
+      <c r="Y103">
+        <v>4</v>
+      </c>
+      <c r="AC103">
+        <v>5</v>
+      </c>
+      <c r="AF103">
+        <v>5</v>
+      </c>
+      <c r="AJ103">
+        <v>5</v>
+      </c>
+      <c r="AL103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>7171</v>
+      </c>
+      <c r="E104">
+        <v>3</v>
+      </c>
+      <c r="G104">
+        <v>3</v>
+      </c>
+      <c r="J104">
+        <v>3</v>
+      </c>
+      <c r="L104">
+        <v>3</v>
+      </c>
+      <c r="O104">
+        <v>3</v>
+      </c>
+      <c r="P104">
+        <v>3</v>
+      </c>
+      <c r="R104">
+        <v>3</v>
+      </c>
+      <c r="T104">
+        <v>4</v>
+      </c>
+      <c r="V104">
+        <v>4</v>
+      </c>
+      <c r="W104">
+        <v>4</v>
+      </c>
+      <c r="X104">
+        <v>5</v>
+      </c>
+      <c r="Z104">
+        <v>5</v>
+      </c>
+      <c r="AB104">
+        <v>5</v>
+      </c>
+      <c r="AE104">
+        <v>5</v>
+      </c>
+      <c r="AH104">
+        <v>2</v>
+      </c>
+      <c r="AJ104">
+        <v>4</v>
+      </c>
+      <c r="AK104">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final execution of UserbasedRecommendations
</commit_message>
<xml_diff>
--- a/DATASET/DATASET.xlsx
+++ b/DATASET/DATASET.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainashastri/Dropbox/sts-workspace/CMPE-239/CMPE-239_RecommenderSystems/DATASET/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainashastri/Desktop/239/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data-org" sheetId="4" r:id="rId1"/>
@@ -130,9 +130,6 @@
     <t>Zootopia</t>
   </si>
   <si>
-    <t>MI</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>Negative Average</t>
+  </si>
+  <si>
+    <t>Mission Impossible</t>
   </si>
 </sst>
 </file>
@@ -272,7 +272,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,6 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -567,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN44"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,25 +672,25 @@
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="AM1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AN1" s="1"/>
     </row>
@@ -3992,8 +3993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE14" sqref="A14:XFD14"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4101,28 +4102,28 @@
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -7685,8 +7686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7796,25 +7797,25 @@
         <v>31</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="19" x14ac:dyDescent="0.25">
@@ -14405,8 +14406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:AL104"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14514,25 +14515,25 @@
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="AM1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AN1" s="1"/>
     </row>
@@ -21857,8 +21858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN104"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="AC14" sqref="A14:XFD14"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21964,28 +21965,28 @@
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="AN1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -28863,7 +28864,7 @@
       <c r="R87">
         <v>1</v>
       </c>
-      <c r="S87">
+      <c r="S87" s="6">
         <v>4</v>
       </c>
       <c r="T87">
@@ -30134,8 +30135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH85" sqref="AH85"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30246,25 +30247,25 @@
         <v>31</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="19" x14ac:dyDescent="0.25">
@@ -43140,7 +43141,10 @@
         <f>IF(NUAverage!E86&gt;0,SUM(NUAverage!E86,NUAverage!$AN86),"")</f>
         <v>1.3076923076923075</v>
       </c>
-      <c r="F86" s="1"/>
+      <c r="F86" s="1">
+        <f>IF(NUAverage!F86&gt;0,SUM(NUAverage!F86,NUAverage!$AN86),"")</f>
+        <v>-1.6923076923076925</v>
+      </c>
       <c r="G86" s="1">
         <f>IF(NUAverage!G86&gt;0,SUM(NUAverage!G86,NUAverage!$AN86),"")</f>
         <v>-0.69230769230769251</v>
@@ -43290,7 +43294,10 @@
         <f>IF(NUAverage!E87&gt;0,SUM(NUAverage!E87,NUAverage!$AN87),"")</f>
         <v/>
       </c>
-      <c r="F87" s="1"/>
+      <c r="F87" s="1" t="str">
+        <f>IF(NUAverage!F87&gt;0,SUM(NUAverage!F87,NUAverage!$AN87),"")</f>
+        <v/>
+      </c>
       <c r="G87" s="1" t="str">
         <f>IF(NUAverage!G87&gt;0,SUM(NUAverage!G87,NUAverage!$AN87),"")</f>
         <v/>
@@ -43440,7 +43447,10 @@
         <f>IF(NUAverage!E88&gt;0,SUM(NUAverage!E88,NUAverage!$AN88),"")</f>
         <v>-1.7200000000000002</v>
       </c>
-      <c r="F88" s="1"/>
+      <c r="F88" s="1" t="str">
+        <f>IF(NUAverage!F88&gt;0,SUM(NUAverage!F88,NUAverage!$AN88),"")</f>
+        <v/>
+      </c>
       <c r="G88" s="1">
         <f>IF(NUAverage!G88&gt;0,SUM(NUAverage!G88,NUAverage!$AN88),"")</f>
         <v>-0.7200000000000002</v>
@@ -43590,7 +43600,10 @@
         <f>IF(NUAverage!E89&gt;0,SUM(NUAverage!E89,NUAverage!$AN89),"")</f>
         <v/>
       </c>
-      <c r="F89" s="1"/>
+      <c r="F89" s="1" t="str">
+        <f>IF(NUAverage!F89&gt;0,SUM(NUAverage!F89,NUAverage!$AN89),"")</f>
+        <v/>
+      </c>
       <c r="G89" s="1" t="str">
         <f>IF(NUAverage!G89&gt;0,SUM(NUAverage!G89,NUAverage!$AN89),"")</f>
         <v/>
@@ -43740,7 +43753,10 @@
         <f>IF(NUAverage!E90&gt;0,SUM(NUAverage!E90,NUAverage!$AN90),"")</f>
         <v/>
       </c>
-      <c r="F90" s="1"/>
+      <c r="F90" s="1">
+        <f>IF(NUAverage!F90&gt;0,SUM(NUAverage!F90,NUAverage!$AN90),"")</f>
+        <v>-0.89999999999999991</v>
+      </c>
       <c r="G90" s="1">
         <f>IF(NUAverage!G90&gt;0,SUM(NUAverage!G90,NUAverage!$AN90),"")</f>
         <v>-0.89999999999999991</v>
@@ -43890,7 +43906,7 @@
         <f>IF(NUAverage!E91&gt;0,SUM(NUAverage!E91,NUAverage!$AN91),"")</f>
         <v>-6.25E-2</v>
       </c>
-      <c r="F91" s="1"/>
+      <c r="F91" s="9"/>
       <c r="G91" s="1" t="str">
         <f>IF(NUAverage!G91&gt;0,SUM(NUAverage!G91,NUAverage!$AN91),"")</f>
         <v/>
@@ -44040,7 +44056,10 @@
         <f>IF(NUAverage!E92&gt;0,SUM(NUAverage!E92,NUAverage!$AN92),"")</f>
         <v>1.2999999999999998</v>
       </c>
-      <c r="F92" s="1"/>
+      <c r="F92" s="1" t="str">
+        <f>IF(NUAverage!F92&gt;0,SUM(NUAverage!F92,NUAverage!$AN92),"")</f>
+        <v/>
+      </c>
       <c r="G92" s="1">
         <f>IF(NUAverage!G92&gt;0,SUM(NUAverage!G92,NUAverage!$AN92),"")</f>
         <v>1.2999999999999998</v>
@@ -44190,7 +44209,10 @@
         <f>IF(NUAverage!E93&gt;0,SUM(NUAverage!E93,NUAverage!$AN93),"")</f>
         <v>0.28571428571428559</v>
       </c>
-      <c r="F93" s="1"/>
+      <c r="F93" s="1">
+        <f>IF(NUAverage!F93&gt;0,SUM(NUAverage!F93,NUAverage!$AN93),"")</f>
+        <v>-0.71428571428571441</v>
+      </c>
       <c r="G93" s="1">
         <f>IF(NUAverage!G93&gt;0,SUM(NUAverage!G93,NUAverage!$AN93),"")</f>
         <v>-1.7142857142857144</v>
@@ -44340,7 +44362,10 @@
         <f>IF(NUAverage!E94&gt;0,SUM(NUAverage!E94,NUAverage!$AN94),"")</f>
         <v>-1.3888888888888888</v>
       </c>
-      <c r="F94" s="1"/>
+      <c r="F94" s="1">
+        <f>IF(NUAverage!F94&gt;0,SUM(NUAverage!F94,NUAverage!$AN94),"")</f>
+        <v>-0.38888888888888884</v>
+      </c>
       <c r="G94" s="1">
         <f>IF(NUAverage!G94&gt;0,SUM(NUAverage!G94,NUAverage!$AN94),"")</f>
         <v>-1.3888888888888888</v>
@@ -44490,7 +44515,10 @@
         <f>IF(NUAverage!E95&gt;0,SUM(NUAverage!E95,NUAverage!$AN95),"")</f>
         <v/>
       </c>
-      <c r="F95" s="1"/>
+      <c r="F95" s="1" t="str">
+        <f>IF(NUAverage!F95&gt;0,SUM(NUAverage!F95,NUAverage!$AN95),"")</f>
+        <v/>
+      </c>
       <c r="G95" s="1" t="str">
         <f>IF(NUAverage!G95&gt;0,SUM(NUAverage!G95,NUAverage!$AN95),"")</f>
         <v/>
@@ -44640,7 +44668,10 @@
         <f>IF(NUAverage!E96&gt;0,SUM(NUAverage!E96,NUAverage!$AN96),"")</f>
         <v/>
       </c>
-      <c r="F96" s="1"/>
+      <c r="F96" s="1">
+        <f>IF(NUAverage!F96&gt;0,SUM(NUAverage!F96,NUAverage!$AN96),"")</f>
+        <v>-0.25</v>
+      </c>
       <c r="G96" s="1" t="str">
         <f>IF(NUAverage!G96&gt;0,SUM(NUAverage!G96,NUAverage!$AN96),"")</f>
         <v/>
@@ -44790,7 +44821,10 @@
         <f>IF(NUAverage!E97&gt;0,SUM(NUAverage!E97,NUAverage!$AN97),"")</f>
         <v>1.4285714285714284</v>
       </c>
-      <c r="F97" s="1"/>
+      <c r="F97" s="1">
+        <f>IF(NUAverage!F97&gt;0,SUM(NUAverage!F97,NUAverage!$AN97),"")</f>
+        <v>1.4285714285714284</v>
+      </c>
       <c r="G97" s="1">
         <f>IF(NUAverage!G97&gt;0,SUM(NUAverage!G97,NUAverage!$AN97),"")</f>
         <v>1.4285714285714284</v>
@@ -44940,7 +44974,10 @@
         <f>IF(NUAverage!E98&gt;0,SUM(NUAverage!E98,NUAverage!$AN98),"")</f>
         <v>1.2999999999999998</v>
       </c>
-      <c r="F98" s="1"/>
+      <c r="F98" s="1">
+        <f>IF(NUAverage!F98&gt;0,SUM(NUAverage!F98,NUAverage!$AN98),"")</f>
+        <v>0.29999999999999982</v>
+      </c>
       <c r="G98" s="1" t="str">
         <f>IF(NUAverage!G98&gt;0,SUM(NUAverage!G98,NUAverage!$AN98),"")</f>
         <v/>
@@ -45090,7 +45127,10 @@
         <f>IF(NUAverage!E99&gt;0,SUM(NUAverage!E99,NUAverage!$AN99),"")</f>
         <v/>
       </c>
-      <c r="F99" s="1"/>
+      <c r="F99" s="1" t="str">
+        <f>IF(NUAverage!F99&gt;0,SUM(NUAverage!F99,NUAverage!$AN99),"")</f>
+        <v/>
+      </c>
       <c r="G99" s="1">
         <f>IF(NUAverage!G99&gt;0,SUM(NUAverage!G99,NUAverage!$AN99),"")</f>
         <v>0.42857142857142838</v>
@@ -45240,7 +45280,10 @@
         <f>IF(NUAverage!E100&gt;0,SUM(NUAverage!E100,NUAverage!$AN100),"")</f>
         <v/>
       </c>
-      <c r="F100" s="1"/>
+      <c r="F100" s="1" t="str">
+        <f>IF(NUAverage!F100&gt;0,SUM(NUAverage!F100,NUAverage!$AN100),"")</f>
+        <v/>
+      </c>
       <c r="G100" s="1">
         <f>IF(NUAverage!G100&gt;0,SUM(NUAverage!G100,NUAverage!$AN100),"")</f>
         <v>0.77777777777777768</v>
@@ -45390,7 +45433,10 @@
         <f>IF(NUAverage!E101&gt;0,SUM(NUAverage!E101,NUAverage!$AN101),"")</f>
         <v>1.5652173913043477</v>
       </c>
-      <c r="F101" s="1"/>
+      <c r="F101" s="1" t="str">
+        <f>IF(NUAverage!F101&gt;0,SUM(NUAverage!F101,NUAverage!$AN101),"")</f>
+        <v/>
+      </c>
       <c r="G101" s="1">
         <f>IF(NUAverage!G101&gt;0,SUM(NUAverage!G101,NUAverage!$AN101),"")</f>
         <v>-0.43478260869565233</v>
@@ -45540,7 +45586,10 @@
         <f>IF(NUAverage!E102&gt;0,SUM(NUAverage!E102,NUAverage!$AN102),"")</f>
         <v>0.15384615384615374</v>
       </c>
-      <c r="F102" s="1"/>
+      <c r="F102" s="1" t="str">
+        <f>IF(NUAverage!F102&gt;0,SUM(NUAverage!F102,NUAverage!$AN102),"")</f>
+        <v/>
+      </c>
       <c r="G102" s="1">
         <f>IF(NUAverage!G102&gt;0,SUM(NUAverage!G102,NUAverage!$AN102),"")</f>
         <v>-1.8461538461538463</v>
@@ -45690,7 +45739,10 @@
         <f>IF(NUAverage!E103&gt;0,SUM(NUAverage!E103,NUAverage!$AN103),"")</f>
         <v/>
       </c>
-      <c r="F103" s="1"/>
+      <c r="F103" s="1">
+        <f>IF(NUAverage!F103&gt;0,SUM(NUAverage!F103,NUAverage!$AN103),"")</f>
+        <v>-9.9999999999999645E-2</v>
+      </c>
       <c r="G103" s="1" t="str">
         <f>IF(NUAverage!G103&gt;0,SUM(NUAverage!G103,NUAverage!$AN103),"")</f>
         <v/>
@@ -45840,7 +45892,10 @@
         <f>IF(NUAverage!E104&gt;0,SUM(NUAverage!E104,NUAverage!$AN104),"")</f>
         <v>-0.70588235294117663</v>
       </c>
-      <c r="F104" s="1"/>
+      <c r="F104" s="1" t="str">
+        <f>IF(NUAverage!F104&gt;0,SUM(NUAverage!F104,NUAverage!$AN104),"")</f>
+        <v/>
+      </c>
       <c r="G104" s="1">
         <f>IF(NUAverage!G104&gt;0,SUM(NUAverage!G104,NUAverage!$AN104),"")</f>
         <v>-0.70588235294117663</v>

</xml_diff>